<commit_message>
finished trainNetwork(), working slowly on backpropagation()
</commit_message>
<xml_diff>
--- a/normalizedData.xlsx
+++ b/normalizedData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Repositories\irregularVolumeNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58F7EC2-3CED-49C7-B627-53BB5389B7EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C468A66-838B-4A2F-AF2D-79C11BA20D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2094,7 +2094,7 @@
   <dimension ref="A1:Z1476"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A185" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E206" sqref="E206"/>
+      <selection activeCell="H185" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>